<commit_message>
Site updated: 2024-04-10 21:19:15
</commit_message>
<xml_diff>
--- a/2024/03/22/c1-listening-01-job-interview/Transcript_完整词汇表.xlsx
+++ b/2024/03/22/c1-listening-01-job-interview/Transcript_完整词汇表.xlsx
@@ -496,18 +496,9 @@
     <t>covered</t>
   </si>
   <si>
-    <t>currently</t>
-  </si>
-  <si>
     <t>cv</t>
   </si>
   <si>
-    <t>follower</t>
-  </si>
-  <si>
-    <t>fully</t>
-  </si>
-  <si>
     <t>hr</t>
   </si>
   <si>
@@ -524,6 +515,15 @@
   </si>
   <si>
     <t>maria</t>
+  </si>
+  <si>
+    <t>preconceive</t>
+  </si>
+  <si>
+    <t>provider</t>
+  </si>
+  <si>
+    <t>um</t>
   </si>
 </sst>
 </file>
@@ -1604,46 +1604,100 @@
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>overview</t>
-        </is>
-      </c>
-      <c r="B27" s="7" t="inlineStr">
-        <is>
-          <t>[ˈəʊvəvjuː]</t>
-        </is>
-      </c>
-      <c r="C27" s="7" t="inlineStr">
-        <is>
-          <t>[ˈoʊvərvjuː]</t>
-        </is>
-      </c>
+          <t>currently</t>
+        </is>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="7" t="inlineStr">
         <is>
-          <t>n. [图情] 综述；概观</t>
+          <t>ad.普遍地；当前</t>
         </is>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
         <is>
+          <t>follower</t>
+        </is>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>n.契据的附面；从动件</t>
+        </is>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>fully</t>
+        </is>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>adv.完全，彻底</t>
+        </is>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>overview</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="inlineStr">
+        <is>
+          <t>[ˈəʊvəvjuː]</t>
+        </is>
+      </c>
+      <c r="C30" s="7" t="inlineStr">
+        <is>
+          <t>[ˈoʊvərvjuː]</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>n. [图情] 综述；概观</t>
+        </is>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
           <t>replicate</t>
         </is>
       </c>
-      <c r="B28" s="7" t="inlineStr">
+      <c r="B31" s="7" t="inlineStr">
         <is>
           <t>[ˈreplɪkeɪt]</t>
         </is>
       </c>
-      <c r="C28" s="7" t="inlineStr">
+      <c r="C31" s="7" t="inlineStr">
         <is>
           <t>[ˈreplɪkeɪt]</t>
         </is>
       </c>
-      <c r="D28" s="7" t="inlineStr">
+      <c r="D31" s="7" t="inlineStr">
         <is>
           <t>n. 复制品；八音阶间隔的反覆音 ;vt. 复制；折叠@@ -1651,9 +1705,45 @@
 ;vi. 重复；折转</t>
         </is>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="n">
-        <v>1.0</v>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>successfully</t>
+        </is>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7" t="inlineStr">
+        <is>
+          <t>ad.成功地</t>
+        </is>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>thanks</t>
+        </is>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7" t="inlineStr">
+        <is>
+          <t>n.感谢 int.谢谢</t>
+        </is>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8" t="n">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>
@@ -7350,7 +7440,7 @@
         <v>153</v>
       </c>
       <c r="F5" s="8" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7364,7 +7454,7 @@
         <v>153</v>
       </c>
       <c r="F6" s="8" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7406,7 +7496,7 @@
         <v>153</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -7420,7 +7510,7 @@
         <v>153</v>
       </c>
       <c r="F10" s="8" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -7434,7 +7524,7 @@
         <v>153</v>
       </c>
       <c r="F11" s="8" t="n">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -7448,7 +7538,7 @@
         <v>153</v>
       </c>
       <c r="F12" s="8" t="n">
-        <v>15.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -7462,7 +7552,7 @@
         <v>153</v>
       </c>
       <c r="F13" s="8" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -7476,96 +7566,6 @@
         <v>153</v>
       </c>
       <c r="F14" s="8" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="inlineStr">
-        <is>
-          <t>preconceive</t>
-        </is>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8" t="inlineStr">
-        <is>
-          <t>其他</t>
-        </is>
-      </c>
-      <c r="F15" s="8" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8" t="inlineStr">
-        <is>
-          <t>其他</t>
-        </is>
-      </c>
-      <c r="F16" s="8" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="inlineStr">
-        <is>
-          <t>successfully</t>
-        </is>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>其他</t>
-        </is>
-      </c>
-      <c r="F17" s="8" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="inlineStr">
-        <is>
-          <t>thanks</t>
-        </is>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8" t="inlineStr">
-        <is>
-          <t>其他</t>
-        </is>
-      </c>
-      <c r="F18" s="8" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="inlineStr">
-        <is>
-          <t>um</t>
-        </is>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8" t="inlineStr">
-        <is>
-          <t>其他</t>
-        </is>
-      </c>
-      <c r="F19" s="8" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>